<commit_message>
Add support for single object sheets
</commit_message>
<xml_diff>
--- a/resources/test.xlsx
+++ b/resources/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="2980" windowWidth="33540" windowHeight="19280" tabRatio="500"/>
+    <workbookView xWindow="5880" yWindow="2980" windowWidth="33540" windowHeight="19280" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="test.json" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="test.json#properties" sheetId="3" r:id="rId3"/>
     <sheet name="Source" sheetId="4" r:id="rId4"/>
     <sheet name="foo.json" sheetId="5" r:id="rId5"/>
+    <sheet name="bar.json@" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>id</t>
   </si>
@@ -155,6 +156,30 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>ignored</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>foo.baz</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>foo.bar</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>array@</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
   </si>
 </sst>
 </file>
@@ -188,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -201,6 +226,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,7 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1101,4 +1127,64 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>